<commit_message>
dataprovider, excel, page object model, properties
</commit_message>
<xml_diff>
--- a/AutomationFramework/src/test/resources/testdata/OpenEmrData.xlsx
+++ b/AutomationFramework/src/test/resources/testdata/OpenEmrData.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="6825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="6825" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="checkVersionNumberTest" sheetId="3" r:id="rId2"/>
+    <sheet name="checkLanguageTest" sheetId="2" r:id="rId3"/>
+    <sheet name="addPatientTest" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Password</t>
   </si>
@@ -48,6 +51,87 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>bala</t>
+  </si>
+  <si>
+    <t>bala123</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>john123</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>ExpectedLanguage</t>
+  </si>
+  <si>
+    <t>Albanian</t>
+  </si>
+  <si>
+    <t>Amharic</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>Armenian</t>
+  </si>
+  <si>
+    <t>Expected Version</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>accountant</t>
+  </si>
+  <si>
+    <t>Version Number: v6.0.0 (2)</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>First Nme</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Expected Alert</t>
+  </si>
+  <si>
+    <t>Expected Patient Detail</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Wick</t>
+  </si>
+  <si>
+    <t>2021-12-16</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Tobacco</t>
+  </si>
+  <si>
+    <t>Medical Record Dashboard - John Wick</t>
   </si>
 </sst>
 </file>
@@ -83,8 +167,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +492,229 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>